<commit_message>
update Readme.md with images
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -1803,7 +1803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5437"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -47274,7 +47274,7 @@
       <c r="F57" s="47"/>
       <c r="G57" s="47"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A58" s="21" t="s">
         <v>44</v>
       </c>
@@ -64859,8 +64859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -65139,11 +65139,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="C2:C3" r:id="rId2" display="a@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>